<commit_message>
update profiles and examples
</commit_message>
<xml_diff>
--- a/StructureDefinition-be-mycareneteagreementdemand.xlsx
+++ b/StructureDefinition-be-mycareneteagreementdemand.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9460" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9460" uniqueCount="273">
   <si>
     <t>Path</t>
   </si>
@@ -735,7 +735,7 @@
 This outcome is not used for error responses in batch/transaction, only for hints and warnings. In a batch operation, the error will be in Bundle.entry.response, and for transaction, there will be a single OperationOutcome instead of a bundle in the case of an error.</t>
   </si>
   <si>
-    <t>messageheader</t>
+    <t>messageHeader</t>
   </si>
   <si>
     <t xml:space="preserve">MessageHeader {https://www.ehealth.fgov.be/standards/fhir/StructureDefinition/be-mycareneteagreementmessageheader}
@@ -800,7 +800,7 @@
     <t>Entity. Role, or Act</t>
   </si>
   <si>
-    <t>practitionerrole</t>
+    <t>practitionerRole</t>
   </si>
   <si>
     <t xml:space="preserve">PractitionerRole {https://www.ehealth.fgov.be/standards/fhir/StructureDefinition/be-practitionerrole}
@@ -844,6 +844,26 @@
   </si>
   <si>
     <t>patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SubjectOfCare Client Resident
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient {https://www.ehealth.fgov.be/standards/fhir/StructureDefinition/be-patient}
+</t>
+  </si>
+  <si>
+    <t>Information about an individual or animal receiving health care services</t>
+  </si>
+  <si>
+    <t>Demographics and other administrative information about an individual or animal receiving care or other health-related services.</t>
+  </si>
+  <si>
+    <t>Patient[classCode=PAT]</t>
+  </si>
+  <si>
+    <t>ClinicalDocument.recordTarget.patientRole</t>
   </si>
   <si>
     <t>Bundle.signature</t>
@@ -1021,7 +1041,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="38.17578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="15.12890625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="15.55859375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="47.5078125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
@@ -28203,11 +28223,11 @@
       </c>
       <c r="B247" s="2"/>
       <c r="C247" t="s" s="2">
-        <v>40</v>
+        <v>261</v>
       </c>
       <c r="D247" s="2"/>
       <c r="E247" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F247" t="s" s="2">
         <v>49</v>
@@ -28219,16 +28239,16 @@
         <v>40</v>
       </c>
       <c r="I247" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J247" t="s" s="2">
-        <v>154</v>
+        <v>262</v>
       </c>
       <c r="K247" t="s" s="2">
-        <v>155</v>
+        <v>263</v>
       </c>
       <c r="L247" t="s" s="2">
-        <v>156</v>
+        <v>264</v>
       </c>
       <c r="M247" s="2"/>
       <c r="N247" s="2"/>
@@ -28291,16 +28311,16 @@
         <v>40</v>
       </c>
       <c r="AI247" t="s" s="2">
-        <v>40</v>
+        <v>231</v>
       </c>
       <c r="AJ247" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK247" t="s" s="2">
-        <v>40</v>
+        <v>265</v>
       </c>
       <c r="AL247" t="s" s="2">
-        <v>40</v>
+        <v>266</v>
       </c>
       <c r="AM247" t="s" s="2">
         <v>40</v>
@@ -31063,7 +31083,7 @@
     </row>
     <row r="273" hidden="true">
       <c r="A273" t="s" s="2">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B273" s="2"/>
       <c r="C273" t="s" s="2">
@@ -31086,19 +31106,19 @@
         <v>50</v>
       </c>
       <c r="J273" t="s" s="2">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="K273" t="s" s="2">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="L273" t="s" s="2">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="M273" t="s" s="2">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="N273" t="s" s="2">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="O273" t="s" s="2">
         <v>40</v>
@@ -31147,7 +31167,7 @@
         <v>40</v>
       </c>
       <c r="AE273" t="s" s="2">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="AF273" t="s" s="2">
         <v>41</v>

</xml_diff>